<commit_message>
commit sembra funzionante pulizie
</commit_message>
<xml_diff>
--- a/Database/richieste_prodotti.xlsx
+++ b/Database/richieste_prodotti.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,16 +519,432 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>2025-12-17 13:28:56</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:31:36</t>
         </is>
       </c>
       <c r="L2" t="n">
         <v>422</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>18</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CERCA 1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Veline</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:31:58</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>18</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>CERCA 1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>LavaWater</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:32:38</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>65</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Rainusso</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>appartamento</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Mocio con bastone e secchio, Scopa, Paletta, Sacchi del patume per clienti</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:39:56</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>BUON PASTORE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Lavapavimenti, Spugne, LavaWater</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2025-12-17 14:24:34</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CERCA 1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>appartamento</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Sacchi del patume per clienti, Pastiglie lavastoviglie per clienti</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2025-12-17 14:25:18</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:22:20</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>65</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Rainusso</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>📝 ttttt</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:11:41</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>65</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Rainusso</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Lavapavimenti, Spugne</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:23:05</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:28:01</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>65</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Rainusso</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Lavapavimenti, Spugne</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:29:30</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:29:33</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5783861406</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Oooo Vvvvv</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>65</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Rainusso</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>pulizie</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Spugne, Lavapavimenti</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2025-12-17 15:58:00</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>